<commit_message>
Power board schematic almost finished
</commit_message>
<xml_diff>
--- a/Hardware/Specification/Connector_Pin_Mapping.xlsx
+++ b/Hardware/Specification/Connector_Pin_Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandru Zirnea\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\BLDC Platform\Hardware\Specification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{888A7011-6C8F-4879-B603-049BC7CB8027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2AF825-65EB-4055-A464-653F0490740D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="15820" xr2:uid="{0F0BE7A8-7224-4495-A7C7-A5E65C3E7885}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="13492" xr2:uid="{0F0BE7A8-7224-4495-A7C7-A5E65C3E7885}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Board side view</t>
   </si>
@@ -123,9 +123,6 @@
     <t>IPHC</t>
   </si>
   <si>
-    <t>VREF</t>
-  </si>
-  <si>
     <t>VBUS</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>SCK</t>
   </si>
   <si>
-    <t>EN_GATE</t>
-  </si>
-  <si>
     <t>CS</t>
   </si>
   <si>
@@ -156,13 +150,22 @@
     <t>MISO</t>
   </si>
   <si>
-    <t>FAULT</t>
-  </si>
-  <si>
-    <t>TX/CS2</t>
-  </si>
-  <si>
     <t>Female connector</t>
+  </si>
+  <si>
+    <t>CS2</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>RST</t>
+  </si>
+  <si>
+    <t>GPIO</t>
   </si>
 </sst>
 </file>
@@ -262,24 +265,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -299,7 +302,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Temă Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -597,213 +600,213 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5AB70D8-012F-4593-90C5-FD88F055AA1A}">
   <dimension ref="A1:AZ52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="7" max="26" width="10.6328125" customWidth="1"/>
+    <col min="7" max="26" width="10.61328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E1" s="4" t="s">
+    <row r="1" spans="1:52" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
     </row>
-    <row r="2" spans="1:52" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
+    <row r="2" spans="1:52" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
     </row>
-    <row r="3" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:52" s="2" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:52" s="2" customFormat="1" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I6" s="2">
+        <v>6</v>
+      </c>
+      <c r="J6" s="2">
+        <v>8</v>
+      </c>
+      <c r="K6" s="2">
+        <v>10</v>
+      </c>
+      <c r="L6" s="2">
+        <v>12</v>
+      </c>
+      <c r="M6" s="2">
+        <v>14</v>
+      </c>
+      <c r="N6" s="2">
+        <v>16</v>
+      </c>
+      <c r="O6" s="2">
+        <v>18</v>
+      </c>
+      <c r="P6" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>22</v>
+      </c>
+      <c r="R6" s="2">
+        <v>24</v>
+      </c>
+      <c r="S6" s="2">
+        <v>26</v>
+      </c>
+      <c r="T6" s="2">
+        <v>28</v>
+      </c>
+      <c r="U6" s="2">
+        <v>30</v>
+      </c>
+      <c r="V6" s="2">
+        <v>32</v>
+      </c>
+      <c r="W6" s="2">
+        <v>34</v>
+      </c>
+      <c r="X6" s="2">
+        <v>36</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>38</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:52" s="1" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+    </row>
+    <row r="8" spans="1:52" ht="40" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="2">
-        <v>4</v>
-      </c>
-      <c r="K6" s="2">
-        <v>5</v>
-      </c>
-      <c r="L6" s="2">
-        <v>6</v>
-      </c>
-      <c r="M6" s="2">
-        <v>7</v>
-      </c>
-      <c r="N6" s="2">
-        <v>8</v>
-      </c>
-      <c r="O6" s="2">
-        <v>9</v>
-      </c>
-      <c r="P6" s="2">
-        <v>10</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>11</v>
-      </c>
-      <c r="R6" s="2">
-        <v>12</v>
-      </c>
-      <c r="S6" s="2">
-        <v>13</v>
-      </c>
-      <c r="T6" s="2">
-        <v>14</v>
-      </c>
-      <c r="U6" s="2">
-        <v>15</v>
-      </c>
-      <c r="V6" s="2">
-        <v>16</v>
-      </c>
-      <c r="W6" s="2">
-        <v>17</v>
-      </c>
-      <c r="X6" s="2">
-        <v>18</v>
-      </c>
-      <c r="Y6" s="2">
-        <v>19</v>
-      </c>
-      <c r="Z6" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:52" s="1" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-    </row>
-    <row r="8" spans="1:52" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="N8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="P8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="R8" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="S8" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="T8" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="U8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="V8" s="9" t="s">
+      <c r="S8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="V8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W8" s="9" t="s">
+      <c r="W8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="X8" s="9" t="s">
+      <c r="X8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Y8" s="9" t="s">
+      <c r="Y8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Z8" s="9" t="s">
+      <c r="Z8" s="5" t="s">
         <v>21</v>
       </c>
       <c r="AA8" s="1"/>
@@ -833,74 +836,74 @@
       <c r="AY8" s="1"/>
       <c r="AZ8" s="1"/>
     </row>
-    <row r="9" spans="1:52" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:52" ht="40" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="L9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M9" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="O9" s="9" t="s">
+      <c r="O9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="9" t="s">
+      <c r="P9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="R9" s="10" t="s">
+      <c r="Q9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="S9" s="9" t="s">
+      <c r="R9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="U9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="T9" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="U9" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="V9" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="W9" s="9" t="s">
+      <c r="V9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="W9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="X9" s="9" t="s">
+      <c r="X9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="Y9" s="9" t="s">
+      <c r="Y9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Z9" s="9" t="s">
-        <v>31</v>
+      <c r="Z9" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
@@ -929,110 +932,110 @@
       <c r="AY9" s="1"/>
       <c r="AZ9" s="1"/>
     </row>
-    <row r="10" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="G10" s="2">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H10" s="2">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="I10" s="2">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="J10" s="2">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="K10" s="2">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="L10" s="2">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="M10" s="2">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="N10" s="2">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="O10" s="2">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="P10" s="2">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="Q10" s="2">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="R10" s="2">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="S10" s="2">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="T10" s="2">
         <v>27</v>
       </c>
       <c r="U10" s="2">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="V10" s="2">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="W10" s="2">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="X10" s="2">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="Y10" s="2">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="Z10" s="2">
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="22" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="23" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="24" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="25" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="26" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="27" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="28" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="29" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="30" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="31" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="32" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="51" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="22" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="23" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="24" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="25" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="26" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="27" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="28" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="29" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="30" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="31" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="32" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="51" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="E1:AD2"/>

</xml_diff>